<commit_message>
Updated version - adjustment to number of peaks located
</commit_message>
<xml_diff>
--- a/Evan/Data_Method_1.xlsx
+++ b/Evan/Data_Method_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessi\Documents\DoD\Evan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jg300416\Documents\MATLAB\DoD\Evan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62802452-BB1D-4EAC-A87C-3BE4E6AA9D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41787FC7-5C00-47CA-9DB6-22DC75B347DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="21600" windowHeight="11385" xr2:uid="{DB4D1D40-A8DA-456B-A30C-81169D4C9387}"/>
+    <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="12735" xr2:uid="{DB4D1D40-A8DA-456B-A30C-81169D4C9387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>p</t>
   </si>
@@ -85,6 +85,78 @@
   </si>
   <si>
     <t>SD_AUC3</t>
+  </si>
+  <si>
+    <t>MCD_Onset3</t>
+  </si>
+  <si>
+    <t>MCD_Offset3</t>
+  </si>
+  <si>
+    <t>MCD_Onset4</t>
+  </si>
+  <si>
+    <t>MCD_Offset4</t>
+  </si>
+  <si>
+    <t>MCD_Onset5</t>
+  </si>
+  <si>
+    <t>MCD_Offset5</t>
+  </si>
+  <si>
+    <t>SD_Onset3</t>
+  </si>
+  <si>
+    <t>SD_Offset3</t>
+  </si>
+  <si>
+    <t>SD_Onset4</t>
+  </si>
+  <si>
+    <t>SD_Offset4</t>
+  </si>
+  <si>
+    <t>SD_Onset5</t>
+  </si>
+  <si>
+    <t>SD_Offset5</t>
+  </si>
+  <si>
+    <t>MCD_AUC1_2</t>
+  </si>
+  <si>
+    <t>SD_AUC1_2</t>
+  </si>
+  <si>
+    <t>MCD_AUC2_3</t>
+  </si>
+  <si>
+    <t>SD_AUC2_3</t>
+  </si>
+  <si>
+    <t>MCD_AUC4</t>
+  </si>
+  <si>
+    <t>SD_AUC4</t>
+  </si>
+  <si>
+    <t>MCD_AUC3_4</t>
+  </si>
+  <si>
+    <t>SD_AUC3_4</t>
+  </si>
+  <si>
+    <t>MCD_AUC5</t>
+  </si>
+  <si>
+    <t>SD_AUC5</t>
+  </si>
+  <si>
+    <t>MCD_AUC4_5</t>
+  </si>
+  <si>
+    <t>SD_AUC4_5</t>
   </si>
 </sst>
 </file>
@@ -442,15 +514,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17343D4B-F7EF-4F82-9097-15B56B1F5001}">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:AO58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q58"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2:AO58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.85546875" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.28515625" customWidth="1"/>
+    <col min="29" max="29" width="12.140625" customWidth="1"/>
+    <col min="30" max="30" width="14.28515625" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" customWidth="1"/>
+    <col min="32" max="32" width="13" customWidth="1"/>
+    <col min="33" max="33" width="14" customWidth="1"/>
+    <col min="34" max="34" width="12.5703125" customWidth="1"/>
+    <col min="35" max="35" width="11.28515625" customWidth="1"/>
+    <col min="36" max="36" width="14.5703125" customWidth="1"/>
+    <col min="37" max="37" width="13.85546875" customWidth="1"/>
+    <col min="38" max="38" width="12.5703125" customWidth="1"/>
+    <col min="39" max="39" width="11.7109375" customWidth="1"/>
+    <col min="40" max="40" width="14.5703125" customWidth="1"/>
+    <col min="41" max="41" width="12.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,37 +578,109 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Y1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Z1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AA1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AE1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -526,37 +703,85 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="I2">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="J2">
+        <v>0.219</v>
+      </c>
+      <c r="N2">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="I2">
+      <c r="O2">
         <v>2.7E-2</v>
       </c>
-      <c r="J2">
+      <c r="P2">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="K2">
+      <c r="Q2">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="L2">
+      <c r="R2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="S2">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="T2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="U2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="V2">
+        <v>0.218</v>
+      </c>
+      <c r="X2">
         <v>195.74737550000003</v>
       </c>
-      <c r="M2">
+      <c r="Y2">
         <v>195.74737550000003</v>
       </c>
-      <c r="N2">
+      <c r="Z2">
         <v>28.480529999999998</v>
       </c>
-      <c r="O2">
+      <c r="AA2">
         <v>28.480529999999998</v>
       </c>
-      <c r="P2">
-        <v>250.17929120000002</v>
-      </c>
-      <c r="Q2">
-        <v>250.17929120000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB2">
+        <v>25.951385700000003</v>
+      </c>
+      <c r="AC2">
+        <v>25.951385700000003</v>
+      </c>
+      <c r="AD2">
+        <v>179.24118049999998</v>
+      </c>
+      <c r="AE2">
+        <v>179.24118049999998</v>
+      </c>
+      <c r="AF2">
+        <v>94.573975349999998</v>
+      </c>
+      <c r="AG2">
+        <v>94.573975349999998</v>
+      </c>
+      <c r="AI2">
+        <v>37.006378249999997</v>
+      </c>
+      <c r="AJ2">
+        <v>895.35904010000013</v>
+      </c>
+      <c r="AK2">
+        <v>126.70898379999998</v>
+      </c>
+      <c r="AO2">
+        <v>722.32055795000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>
@@ -578,38 +803,50 @@
       <c r="G3">
         <v>0.13500000000000001</v>
       </c>
-      <c r="H3">
+      <c r="N3">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="I3">
+      <c r="O3">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="J3">
+      <c r="P3">
         <v>0.11899999999999999</v>
       </c>
-      <c r="K3">
+      <c r="Q3">
         <v>0.122</v>
       </c>
-      <c r="L3">
+      <c r="R3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="S3">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="X3">
         <v>729.12216186523438</v>
       </c>
-      <c r="M3">
+      <c r="Y3">
         <v>501.60598754882813</v>
       </c>
-      <c r="N3">
+      <c r="Z3">
         <v>405.29632568359375</v>
       </c>
-      <c r="O3">
+      <c r="AA3">
         <v>85.895538330078125</v>
       </c>
-      <c r="P3">
-        <v>1837.6388549804688</v>
-      </c>
-      <c r="Q3">
-        <v>1308.2542419433594</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB3">
+        <v>703.22036743164063</v>
+      </c>
+      <c r="AC3">
+        <v>720.75271606445313</v>
+      </c>
+      <c r="AE3">
+        <v>95.52001953125</v>
+      </c>
+      <c r="AG3">
+        <v>223.88076782226563</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
@@ -620,7 +857,7 @@
         <v>73.878200000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
@@ -631,7 +868,7 @@
         <v>65.048100000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14</v>
       </c>
@@ -647,32 +884,32 @@
       <c r="E6">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="H6">
+      <c r="N6">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I6">
+      <c r="O6">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="J6">
+      <c r="P6">
         <v>0.109</v>
       </c>
-      <c r="K6">
+      <c r="Q6">
         <v>0.121</v>
       </c>
-      <c r="L6">
+      <c r="X6">
         <v>154.0069580078125</v>
       </c>
-      <c r="M6">
+      <c r="Y6">
         <v>154.0069580078125</v>
       </c>
-      <c r="O6">
+      <c r="AA6">
         <v>147.27020263671875</v>
       </c>
-      <c r="Q6">
-        <v>955.19256591796875</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AC6">
+        <v>653.9154052734375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
@@ -700,20 +937,32 @@
       <c r="I7">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="L7">
+      <c r="N7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="O7">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="X7">
         <v>88.56964111328125</v>
       </c>
-      <c r="M7">
+      <c r="Y7">
         <v>748.19183349609375</v>
       </c>
-      <c r="N7">
+      <c r="Z7">
         <v>99.582672119140625</v>
       </c>
-      <c r="P7">
-        <v>524.28054809570313</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB7">
+        <v>336.12823486328125</v>
+      </c>
+      <c r="AD7">
+        <v>748.19183349609375</v>
+      </c>
+      <c r="AF7">
+        <v>193.29833984375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16</v>
       </c>
@@ -729,20 +978,20 @@
       <c r="E8">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="H8">
+      <c r="N8">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="I8">
+      <c r="O8">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="L8">
+      <c r="X8">
         <v>65.51361083984375</v>
       </c>
-      <c r="M8">
+      <c r="Y8">
         <v>65.51361083984375</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>17</v>
       </c>
@@ -758,20 +1007,20 @@
       <c r="E9">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="H9">
+      <c r="N9">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="I9">
+      <c r="O9">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="L9">
+      <c r="X9">
         <v>1333.9080810546875</v>
       </c>
-      <c r="M9">
+      <c r="Y9">
         <v>1380.7907104492188</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>18</v>
       </c>
@@ -794,37 +1043,61 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="H10">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="I10">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N10">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="I10">
+      <c r="O10">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="J10">
+      <c r="P10">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="K10">
+      <c r="Q10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="L10">
+      <c r="R10">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="S10">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="X10">
         <v>230.26784261067706</v>
       </c>
-      <c r="M10">
+      <c r="Y10">
         <v>230.26784261067706</v>
       </c>
-      <c r="N10">
+      <c r="Z10">
         <v>1900.2978006998701</v>
       </c>
-      <c r="O10">
+      <c r="AA10">
         <v>1900.2978006998701</v>
       </c>
-      <c r="P10">
-        <v>2216.2310282389321</v>
-      </c>
-      <c r="Q10">
-        <v>2216.2310282389321</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB10">
+        <v>85.665384928385407</v>
+      </c>
+      <c r="AC10">
+        <v>85.665384928385407</v>
+      </c>
+      <c r="AD10">
+        <v>128.60616048177084</v>
+      </c>
+      <c r="AE10">
+        <v>128.60616048177084</v>
+      </c>
+      <c r="AF10">
+        <v>69.033304850260421</v>
+      </c>
+      <c r="AG10">
+        <v>69.033304850260421</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>19</v>
       </c>
@@ -847,37 +1120,109 @@
         <v>5.5E-2</v>
       </c>
       <c r="H11">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="I11">
+        <v>0.124</v>
+      </c>
+      <c r="J11">
+        <v>0.13</v>
+      </c>
+      <c r="K11">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="L11">
+        <v>0.17</v>
+      </c>
+      <c r="M11">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="N11">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I11">
+      <c r="O11">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J11">
+      <c r="P11">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="K11">
+      <c r="Q11">
         <v>5.5E-2</v>
       </c>
-      <c r="L11">
+      <c r="R11">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="S11">
+        <v>0.124</v>
+      </c>
+      <c r="T11">
+        <v>0.13</v>
+      </c>
+      <c r="U11">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="V11">
+        <v>0.186</v>
+      </c>
+      <c r="W11">
+        <v>0.192</v>
+      </c>
+      <c r="X11">
         <v>23.281097412109375</v>
       </c>
-      <c r="M11">
+      <c r="Y11">
         <v>23.281097412109375</v>
       </c>
-      <c r="N11">
+      <c r="Z11">
         <v>210.16693115234375</v>
       </c>
-      <c r="O11">
+      <c r="AA11">
         <v>210.16693115234375</v>
       </c>
-      <c r="P11">
-        <v>323.1658935546875</v>
-      </c>
-      <c r="Q11">
-        <v>323.1658935546875</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB11">
+        <v>89.717864990234375</v>
+      </c>
+      <c r="AC11">
+        <v>89.717864990234375</v>
+      </c>
+      <c r="AD11">
+        <v>460.84976196289063</v>
+      </c>
+      <c r="AE11">
+        <v>453.2928466796875</v>
+      </c>
+      <c r="AF11">
+        <v>142.75741577148438</v>
+      </c>
+      <c r="AG11">
+        <v>150.3143310546875</v>
+      </c>
+      <c r="AH11">
+        <v>85.15167236328125</v>
+      </c>
+      <c r="AI11">
+        <v>32.062530517578125</v>
+      </c>
+      <c r="AJ11">
+        <v>38.421630859375</v>
+      </c>
+      <c r="AK11">
+        <v>38.421630859375</v>
+      </c>
+      <c r="AL11">
+        <v>21.42333984375</v>
+      </c>
+      <c r="AM11">
+        <v>48.48480224609375</v>
+      </c>
+      <c r="AN11">
+        <v>160.08758544921875</v>
+      </c>
+      <c r="AO11">
+        <v>292.95730590820313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20</v>
       </c>
@@ -890,29 +1235,59 @@
       <c r="D12">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="H12">
+      <c r="N12">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="I12">
+      <c r="O12">
         <v>0.121</v>
       </c>
-      <c r="J12">
+      <c r="P12">
         <v>0.13900000000000001</v>
       </c>
-      <c r="K12">
+      <c r="Q12">
         <v>0.14399999999999999</v>
       </c>
-      <c r="M12">
+      <c r="R12">
+        <v>0.155</v>
+      </c>
+      <c r="S12">
+        <v>0.161</v>
+      </c>
+      <c r="T12">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="U12">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="V12">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="Y12">
         <v>6134.4261169433594</v>
       </c>
-      <c r="O12">
+      <c r="AA12">
         <v>104.75540161132813</v>
       </c>
-      <c r="Q12">
-        <v>6543.4303283691406</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AC12">
+        <v>304.24880981445313</v>
+      </c>
+      <c r="AE12">
+        <v>148.03695678710938</v>
+      </c>
+      <c r="AG12">
+        <v>213.73748779296875</v>
+      </c>
+      <c r="AI12">
+        <v>3497.9705810546875</v>
+      </c>
+      <c r="AK12">
+        <v>56.52618408203125</v>
+      </c>
+      <c r="AO12">
+        <v>54.37469482421875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>21</v>
       </c>
@@ -928,20 +1303,20 @@
       <c r="E13">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="H13">
+      <c r="N13">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="I13">
+      <c r="O13">
         <v>5.5E-2</v>
       </c>
-      <c r="L13">
+      <c r="X13">
         <v>3440.2389526367188</v>
       </c>
-      <c r="M13">
+      <c r="Y13">
         <v>3501.1978149414063</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>22</v>
       </c>
@@ -964,37 +1339,61 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="H14">
+        <v>0.104</v>
+      </c>
+      <c r="I14">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="N14">
         <v>3.1E-2</v>
       </c>
-      <c r="I14">
+      <c r="O14">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="J14">
+      <c r="P14">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="K14">
+      <c r="Q14">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="L14">
+      <c r="R14">
+        <v>0.104</v>
+      </c>
+      <c r="S14">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="X14">
         <v>3880.0315856933594</v>
       </c>
-      <c r="M14">
+      <c r="Y14">
         <v>3880.0315856933594</v>
       </c>
-      <c r="N14">
+      <c r="Z14">
         <v>285.88485717773438</v>
       </c>
-      <c r="O14">
+      <c r="AA14">
         <v>285.88485717773438</v>
       </c>
-      <c r="P14">
-        <v>5888.6680603027344</v>
-      </c>
-      <c r="Q14">
-        <v>5888.6680603027344</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB14">
+        <v>1722.7516174316406</v>
+      </c>
+      <c r="AC14">
+        <v>1722.7516174316406</v>
+      </c>
+      <c r="AD14">
+        <v>1516.4680480957031</v>
+      </c>
+      <c r="AE14">
+        <v>1516.4680480957031</v>
+      </c>
+      <c r="AF14">
+        <v>261.8560791015625</v>
+      </c>
+      <c r="AG14">
+        <v>261.8560791015625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>23</v>
       </c>
@@ -1017,37 +1416,73 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="H15">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="I15">
+        <v>0.04</v>
+      </c>
+      <c r="J15">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="K15">
+        <v>6.2E-2</v>
+      </c>
+      <c r="N15">
         <v>1.9E-2</v>
       </c>
-      <c r="I15">
+      <c r="O15">
         <v>2.7E-2</v>
       </c>
-      <c r="J15">
+      <c r="P15">
         <v>3.1E-2</v>
       </c>
-      <c r="K15">
+      <c r="Q15">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="L15">
+      <c r="R15">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="S15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="X15">
         <v>67.081451416015625</v>
       </c>
-      <c r="M15">
+      <c r="Y15">
         <v>67.081451416015625</v>
       </c>
-      <c r="N15">
+      <c r="Z15">
         <v>21.4996337890625</v>
       </c>
-      <c r="O15">
+      <c r="AA15">
         <v>21.4996337890625</v>
       </c>
-      <c r="P15">
-        <v>106.67800903320313</v>
-      </c>
-      <c r="Q15">
-        <v>106.67800903320313</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB15">
+        <v>18.096923828125</v>
+      </c>
+      <c r="AC15">
+        <v>18.096923828125</v>
+      </c>
+      <c r="AD15">
+        <v>28.194427490234375</v>
+      </c>
+      <c r="AE15">
+        <v>212.73040771484375</v>
+      </c>
+      <c r="AF15">
+        <v>14.888763427734375</v>
+      </c>
+      <c r="AG15">
+        <v>14.888763427734375</v>
+      </c>
+      <c r="AH15">
+        <v>137.31765747070313</v>
+      </c>
+      <c r="AJ15">
+        <v>31.77642822265625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>24</v>
       </c>
@@ -1070,37 +1505,109 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="H16">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="J16">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="K16">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="L16">
+        <v>0.187</v>
+      </c>
+      <c r="M16">
+        <v>0.192</v>
+      </c>
+      <c r="N16">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I16">
+      <c r="O16">
         <v>7.8E-2</v>
       </c>
-      <c r="J16">
+      <c r="P16">
         <v>0.15</v>
       </c>
-      <c r="K16">
+      <c r="Q16">
         <v>0.155</v>
       </c>
-      <c r="L16">
+      <c r="R16">
+        <v>0.16</v>
+      </c>
+      <c r="S16">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="T16">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="U16">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="V16">
+        <v>0.187</v>
+      </c>
+      <c r="W16">
+        <v>0.191</v>
+      </c>
+      <c r="X16">
         <v>3382.4539184570313</v>
       </c>
-      <c r="M16">
+      <c r="Y16">
         <v>3371.8414306640625</v>
       </c>
-      <c r="N16">
+      <c r="Z16">
         <v>118.3624267578125</v>
       </c>
-      <c r="O16">
+      <c r="AA16">
         <v>65.8111572265625</v>
       </c>
-      <c r="P16">
-        <v>3831.23779296875</v>
-      </c>
-      <c r="Q16">
-        <v>3976.86767578125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB16">
+        <v>330.42144775390625</v>
+      </c>
+      <c r="AC16">
+        <v>539.215087890625</v>
+      </c>
+      <c r="AD16">
+        <v>278.40423583984375</v>
+      </c>
+      <c r="AE16">
+        <v>63.16375732421875</v>
+      </c>
+      <c r="AF16">
+        <v>29.9224853515625</v>
+      </c>
+      <c r="AG16">
+        <v>55.13763427734375</v>
+      </c>
+      <c r="AH16">
+        <v>83.43505859375</v>
+      </c>
+      <c r="AI16">
+        <v>50.4913330078125</v>
+      </c>
+      <c r="AJ16">
+        <v>32.03582763671875</v>
+      </c>
+      <c r="AK16">
+        <v>99.60174560546875</v>
+      </c>
+      <c r="AL16">
+        <v>75.17242431640625</v>
+      </c>
+      <c r="AM16">
+        <v>65.093994140625</v>
+      </c>
+      <c r="AN16">
+        <v>77.7587890625</v>
+      </c>
+      <c r="AO16">
+        <v>87.53204345703125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>25</v>
       </c>
@@ -1122,38 +1629,38 @@
       <c r="G17">
         <v>0.112</v>
       </c>
-      <c r="H17">
+      <c r="N17">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="I17">
+      <c r="O17">
         <v>3.9E-2</v>
       </c>
-      <c r="J17">
+      <c r="P17">
         <v>0.109</v>
       </c>
-      <c r="K17">
+      <c r="Q17">
         <v>0.112</v>
       </c>
-      <c r="L17">
+      <c r="X17">
         <v>2429.5578002929688</v>
       </c>
-      <c r="M17">
+      <c r="Y17">
         <v>2429.5578002929688</v>
       </c>
-      <c r="N17">
+      <c r="Z17">
         <v>215.61431884765625</v>
       </c>
-      <c r="O17">
+      <c r="AA17">
         <v>215.61431884765625</v>
       </c>
-      <c r="P17">
-        <v>3727.2796630859375</v>
-      </c>
-      <c r="Q17">
-        <v>3727.2796630859375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB17">
+        <v>1082.1075439453125</v>
+      </c>
+      <c r="AC17">
+        <v>1082.1075439453125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>26</v>
       </c>
@@ -1176,37 +1683,73 @@
         <v>0.111</v>
       </c>
       <c r="H18">
+        <v>0.123</v>
+      </c>
+      <c r="I18">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="J18">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="K18">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="L18">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="M18">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="N18">
         <v>1.6E-2</v>
       </c>
-      <c r="I18">
+      <c r="O18">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="J18">
+      <c r="P18">
         <v>0.127</v>
       </c>
-      <c r="K18">
+      <c r="Q18">
         <v>0.13900000000000001</v>
       </c>
-      <c r="L18">
+      <c r="X18">
         <v>3245.17822265625</v>
       </c>
-      <c r="M18">
+      <c r="Y18">
         <v>3245.17822265625</v>
       </c>
-      <c r="N18">
+      <c r="Z18">
         <v>50.14801025390625</v>
       </c>
-      <c r="O18">
+      <c r="AA18">
         <v>149.00970458984375</v>
       </c>
-      <c r="P18">
-        <v>3406.0287475585938</v>
-      </c>
-      <c r="Q18">
-        <v>3647.5906372070313</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB18">
+        <v>110.7025146484375</v>
+      </c>
+      <c r="AC18">
+        <v>253.4027099609375</v>
+      </c>
+      <c r="AD18">
+        <v>179.38995361328125</v>
+      </c>
+      <c r="AF18">
+        <v>62.17193603515625</v>
+      </c>
+      <c r="AH18">
+        <v>24.07073974609375</v>
+      </c>
+      <c r="AJ18">
+        <v>137.359619140625</v>
+      </c>
+      <c r="AL18">
+        <v>23.44512939453125</v>
+      </c>
+      <c r="AN18">
+        <v>302.60467529296875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>27</v>
       </c>
@@ -1229,37 +1772,49 @@
         <v>0.11700000000000001</v>
       </c>
       <c r="H19">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="I19">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="N19">
         <v>0.109</v>
       </c>
-      <c r="I19">
+      <c r="O19">
         <v>0.11600000000000001</v>
       </c>
-      <c r="J19">
+      <c r="P19">
         <v>0.13900000000000001</v>
       </c>
-      <c r="K19">
+      <c r="Q19">
         <v>0.14199999999999999</v>
       </c>
-      <c r="L19">
+      <c r="X19">
         <v>2208.1298828125</v>
       </c>
-      <c r="M19">
+      <c r="Y19">
         <v>2587.738037109375</v>
       </c>
-      <c r="N19">
+      <c r="Z19">
         <v>3066.5435791015625</v>
       </c>
-      <c r="O19">
+      <c r="AA19">
         <v>1059.1278076171875</v>
       </c>
-      <c r="P19">
-        <v>5914.8941040039063</v>
-      </c>
-      <c r="Q19">
-        <v>7323.7533569335938</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB19">
+        <v>640.22064208984375</v>
+      </c>
+      <c r="AC19">
+        <v>3676.8875122070313</v>
+      </c>
+      <c r="AD19">
+        <v>1059.1278076171875</v>
+      </c>
+      <c r="AF19">
+        <v>3504.5089721679688</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>28</v>
       </c>
@@ -1281,38 +1836,38 @@
       <c r="G20">
         <v>0.125</v>
       </c>
-      <c r="H20">
+      <c r="N20">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="I20">
+      <c r="O20">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="J20">
+      <c r="P20">
         <v>0.115</v>
       </c>
-      <c r="K20">
+      <c r="Q20">
         <v>0.125</v>
       </c>
-      <c r="L20">
+      <c r="X20">
         <v>358.8104248046875</v>
       </c>
-      <c r="M20">
+      <c r="Y20">
         <v>358.8104248046875</v>
       </c>
-      <c r="N20">
+      <c r="Z20">
         <v>276.91650390625</v>
       </c>
-      <c r="O20">
+      <c r="AA20">
         <v>276.91650390625</v>
       </c>
-      <c r="P20">
-        <v>1205.1620483398438</v>
-      </c>
-      <c r="Q20">
-        <v>1205.1620483398438</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB20">
+        <v>569.43511962890625</v>
+      </c>
+      <c r="AC20">
+        <v>569.43511962890625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>29</v>
       </c>
@@ -1335,37 +1890,43 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="H21">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="N21">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="I21">
+      <c r="O21">
         <v>0.05</v>
       </c>
-      <c r="J21">
+      <c r="P21">
         <v>0.23799999999999999</v>
       </c>
-      <c r="K21">
+      <c r="Q21">
         <v>0.24399999999999999</v>
       </c>
-      <c r="L21">
+      <c r="X21">
         <v>3148.040771484375</v>
       </c>
-      <c r="M21">
+      <c r="Y21">
         <v>3098.0606079101563</v>
       </c>
-      <c r="N21">
+      <c r="Z21">
         <v>174.407958984375</v>
       </c>
-      <c r="O21">
+      <c r="AA21">
         <v>450.8056640625</v>
       </c>
-      <c r="P21">
-        <v>3457.4203491210938</v>
-      </c>
-      <c r="Q21">
-        <v>7619.44580078125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB21">
+        <v>134.97161865234375</v>
+      </c>
+      <c r="AC21">
+        <v>4070.5795288085938</v>
+      </c>
+      <c r="AF21">
+        <v>3316.0934448242188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>30</v>
       </c>
@@ -1375,29 +1936,29 @@
       <c r="C22">
         <v>6.0216000000000003</v>
       </c>
-      <c r="H22">
+      <c r="N22">
         <v>1.6E-2</v>
       </c>
-      <c r="I22">
+      <c r="O22">
         <v>0.02</v>
       </c>
-      <c r="J22">
+      <c r="P22">
         <v>0.185</v>
       </c>
-      <c r="K22">
+      <c r="Q22">
         <v>0.189</v>
       </c>
-      <c r="M22">
+      <c r="Y22">
         <v>26.78680419921875</v>
       </c>
-      <c r="O22">
+      <c r="AA22">
         <v>24.6429443359375</v>
       </c>
-      <c r="Q22">
-        <v>702.81219482421875</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AC22">
+        <v>651.3824462890625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>31</v>
       </c>
@@ -1413,20 +1974,20 @@
       <c r="E23">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="H23">
+      <c r="N23">
         <v>3.1E-2</v>
       </c>
-      <c r="I23">
+      <c r="O23">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="L23">
+      <c r="X23">
         <v>3870.6436157226563</v>
       </c>
-      <c r="M23">
+      <c r="Y23">
         <v>3845.8786010742188</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>35</v>
       </c>
@@ -1442,32 +2003,44 @@
       <c r="E24">
         <v>5.5E-2</v>
       </c>
-      <c r="H24">
+      <c r="N24">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="I24">
+      <c r="O24">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="J24">
+      <c r="P24">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="K24">
+      <c r="Q24">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="L24">
+      <c r="R24">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="S24">
+        <v>5.5E-2</v>
+      </c>
+      <c r="X24">
         <v>1082.6034545898438</v>
       </c>
-      <c r="M24">
+      <c r="Y24">
         <v>223.50311279296875</v>
       </c>
-      <c r="O24">
+      <c r="AA24">
         <v>220.245361328125</v>
       </c>
-      <c r="Q24">
-        <v>575.5157470703125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AC24">
+        <v>131.76727294921875</v>
+      </c>
+      <c r="AE24">
+        <v>383.0108642578125</v>
+      </c>
+      <c r="AG24">
+        <v>124.07684326171875</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>36</v>
       </c>
@@ -1483,20 +2056,20 @@
       <c r="E25">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="H25">
+      <c r="N25">
         <v>2.7E-2</v>
       </c>
-      <c r="I25">
+      <c r="O25">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="L25">
+      <c r="X25">
         <v>303.45916748046875</v>
       </c>
-      <c r="M25">
+      <c r="Y25">
         <v>303.45916748046875</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>37</v>
       </c>
@@ -1519,37 +2092,49 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="H26">
+        <v>0.245</v>
+      </c>
+      <c r="N26">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="I26">
+      <c r="O26">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="J26">
+      <c r="P26">
         <v>0.222</v>
       </c>
-      <c r="K26">
+      <c r="Q26">
         <v>0.22900000000000001</v>
       </c>
-      <c r="L26">
+      <c r="R26">
+        <v>0.245</v>
+      </c>
+      <c r="X26">
         <v>1475.067138671875</v>
       </c>
-      <c r="M26">
+      <c r="Y26">
         <v>1475.067138671875</v>
       </c>
-      <c r="N26">
+      <c r="Z26">
         <v>524.87945556640625</v>
       </c>
-      <c r="O26">
+      <c r="AA26">
         <v>389.5721435546875</v>
       </c>
-      <c r="P26">
-        <v>3612.9226684570313</v>
-      </c>
-      <c r="Q26">
-        <v>3612.9226684570313</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB26">
+        <v>1612.97607421875</v>
+      </c>
+      <c r="AC26">
+        <v>1748.2833862304688</v>
+      </c>
+      <c r="AF26">
+        <v>419.0673828125</v>
+      </c>
+      <c r="AG26">
+        <v>419.0673828125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>38</v>
       </c>
@@ -1565,20 +2150,20 @@
       <c r="E27">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="H27">
+      <c r="N27">
         <v>3.1E-2</v>
       </c>
-      <c r="I27">
+      <c r="O27">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="L27">
+      <c r="X27">
         <v>2504.2572021484375</v>
       </c>
-      <c r="M27">
+      <c r="Y27">
         <v>2721.37451171875</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>39</v>
       </c>
@@ -1601,37 +2186,61 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="H28">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I28">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="N28">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="I28">
+      <c r="O28">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="J28">
+      <c r="P28">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="K28">
+      <c r="Q28">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="L28">
+      <c r="R28">
+        <v>6.2E-2</v>
+      </c>
+      <c r="S28">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="X28">
         <v>4911.6744995117188</v>
       </c>
-      <c r="M28">
+      <c r="Y28">
         <v>4868.072509765625</v>
       </c>
-      <c r="N28">
+      <c r="Z28">
         <v>162.22381591796875</v>
       </c>
-      <c r="O28">
+      <c r="AA28">
         <v>135.30731201171875</v>
       </c>
-      <c r="P28">
-        <v>5159.1110229492188</v>
-      </c>
-      <c r="Q28">
-        <v>5088.592529296875</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB28">
+        <v>85.21270751953125</v>
+      </c>
+      <c r="AC28">
+        <v>85.21270751953125</v>
+      </c>
+      <c r="AD28">
+        <v>445.03021240234375</v>
+      </c>
+      <c r="AE28">
+        <v>383.72039794921875</v>
+      </c>
+      <c r="AF28">
+        <v>91.28570556640625</v>
+      </c>
+      <c r="AG28">
+        <v>118.20220947265625</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>40</v>
       </c>
@@ -1653,26 +2262,26 @@
       <c r="G29">
         <v>0.14899999999999999</v>
       </c>
-      <c r="H29">
+      <c r="N29">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="I29">
+      <c r="O29">
         <v>5.5E-2</v>
       </c>
-      <c r="L29">
+      <c r="X29">
         <v>1112.7138137817383</v>
       </c>
-      <c r="M29">
+      <c r="Y29">
         <v>1079.4830322265625</v>
       </c>
-      <c r="N29">
+      <c r="Z29">
         <v>288.848876953125</v>
       </c>
-      <c r="P29">
-        <v>2259.4547271728516</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB29">
+        <v>857.89203643798828</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>41</v>
       </c>
@@ -1694,38 +2303,50 @@
       <c r="G30">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="H30">
+      <c r="N30">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="I30">
+      <c r="O30">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="J30">
+      <c r="P30">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="K30">
+      <c r="Q30">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="L30">
+      <c r="R30">
+        <v>0.109</v>
+      </c>
+      <c r="S30">
+        <v>0.114</v>
+      </c>
+      <c r="X30">
         <v>553.1463623046875</v>
       </c>
-      <c r="M30">
+      <c r="Y30">
         <v>553.1463623046875</v>
       </c>
-      <c r="N30">
+      <c r="Z30">
         <v>571.0601806640625</v>
       </c>
-      <c r="O30">
+      <c r="AA30">
         <v>590.8660888671875</v>
       </c>
-      <c r="P30">
-        <v>1144.0811157226563</v>
-      </c>
-      <c r="Q30">
-        <v>1155.426025390625</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB30">
+        <v>19.87457275390625</v>
+      </c>
+      <c r="AC30">
+        <v>11.41357421875</v>
+      </c>
+      <c r="AE30">
+        <v>30.55572509765625</v>
+      </c>
+      <c r="AG30">
+        <v>68.27545166015625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>42</v>
       </c>
@@ -1736,7 +2357,7 @@
         <v>130.35910000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>43</v>
       </c>
@@ -1759,37 +2380,85 @@
         <v>0.11799999999999999</v>
       </c>
       <c r="H32">
+        <v>0.121</v>
+      </c>
+      <c r="I32">
+        <v>0.13</v>
+      </c>
+      <c r="J32">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="K32">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="N32">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="I32">
+      <c r="O32">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="J32">
+      <c r="P32">
         <v>0.112</v>
       </c>
-      <c r="K32">
+      <c r="Q32">
         <v>0.11799999999999999</v>
       </c>
-      <c r="L32">
+      <c r="R32">
+        <v>0.121</v>
+      </c>
+      <c r="S32">
+        <v>0.13</v>
+      </c>
+      <c r="T32">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="U32">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="X32">
         <v>51.85699462890625</v>
       </c>
-      <c r="M32">
+      <c r="Y32">
         <v>58.50982666015625</v>
       </c>
-      <c r="N32">
+      <c r="Z32">
         <v>60.27984619140625</v>
       </c>
-      <c r="O32">
+      <c r="AA32">
         <v>60.27984619140625</v>
       </c>
-      <c r="P32">
-        <v>346.5728759765625</v>
-      </c>
-      <c r="Q32">
-        <v>346.5728759765625</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB32">
+        <v>234.43603515625</v>
+      </c>
+      <c r="AC32">
+        <v>227.783203125</v>
+      </c>
+      <c r="AD32">
+        <v>81.47430419921875</v>
+      </c>
+      <c r="AE32">
+        <v>81.47430419921875</v>
+      </c>
+      <c r="AF32">
+        <v>19.1650390625</v>
+      </c>
+      <c r="AG32">
+        <v>19.1650390625</v>
+      </c>
+      <c r="AH32">
+        <v>65.887451171875</v>
+      </c>
+      <c r="AI32">
+        <v>73.43292236328125</v>
+      </c>
+      <c r="AJ32">
+        <v>65.78826904296875</v>
+      </c>
+      <c r="AK32">
+        <v>58.2427978515625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>44</v>
       </c>
@@ -1805,20 +2474,20 @@
       <c r="E33">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="H33">
+      <c r="N33">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="I33">
+      <c r="O33">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="L33">
+      <c r="X33">
         <v>112.457275390625</v>
       </c>
-      <c r="M33">
+      <c r="Y33">
         <v>112.457275390625</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>45</v>
       </c>
@@ -1834,20 +2503,20 @@
       <c r="E34">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="H34">
+      <c r="N34">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="I34">
+      <c r="O34">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="L34">
+      <c r="X34">
         <v>6103.5079956054688</v>
       </c>
-      <c r="M34">
+      <c r="Y34">
         <v>6103.5079956054688</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>48</v>
       </c>
@@ -1869,38 +2538,38 @@
       <c r="G35">
         <v>0.161</v>
       </c>
-      <c r="H35">
+      <c r="N35">
         <v>0.04</v>
       </c>
-      <c r="I35">
+      <c r="O35">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="J35">
+      <c r="P35">
         <v>0.153</v>
       </c>
-      <c r="K35">
+      <c r="Q35">
         <v>0.161</v>
       </c>
-      <c r="L35">
+      <c r="X35">
         <v>1977.5161743164063</v>
       </c>
-      <c r="M35">
+      <c r="Y35">
         <v>1977.5161743164063</v>
       </c>
-      <c r="N35">
+      <c r="Z35">
         <v>817.9931640625</v>
       </c>
-      <c r="O35">
+      <c r="AA35">
         <v>817.9931640625</v>
       </c>
-      <c r="P35">
-        <v>5155.6777954101563</v>
-      </c>
-      <c r="Q35">
-        <v>5155.6777954101563</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB35">
+        <v>2360.16845703125</v>
+      </c>
+      <c r="AC35">
+        <v>2360.16845703125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>49</v>
       </c>
@@ -1916,20 +2585,20 @@
       <c r="E36">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="H36">
+      <c r="N36">
         <v>0.03</v>
       </c>
-      <c r="I36">
+      <c r="O36">
         <v>6.3E-2</v>
       </c>
-      <c r="L36">
+      <c r="X36">
         <v>1303.6117553710938</v>
       </c>
-      <c r="M36">
+      <c r="Y36">
         <v>1409.5840454101563</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>50</v>
       </c>
@@ -1952,25 +2621,37 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="H37">
-        <v>0.124</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="I37">
         <v>0.127</v>
       </c>
-      <c r="L37">
+      <c r="N37">
+        <v>0.124</v>
+      </c>
+      <c r="O37">
+        <v>0.127</v>
+      </c>
+      <c r="X37">
         <v>51.8341064453125</v>
       </c>
-      <c r="M37">
+      <c r="Y37">
         <v>57.74688720703125</v>
       </c>
-      <c r="N37">
+      <c r="Z37">
         <v>54.2755126953125</v>
       </c>
-      <c r="P37">
-        <v>200.00457763671875</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB37">
+        <v>93.89495849609375</v>
+      </c>
+      <c r="AD37">
+        <v>116.3330078125</v>
+      </c>
+      <c r="AF37">
+        <v>259.01031494140625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>51</v>
       </c>
@@ -1986,20 +2667,20 @@
       <c r="E38">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="H38">
+      <c r="N38">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="I38">
+      <c r="O38">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="L38">
+      <c r="X38">
         <v>41.35894775390625</v>
       </c>
-      <c r="M38">
+      <c r="Y38">
         <v>41.35894775390625</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>52</v>
       </c>
@@ -2015,20 +2696,20 @@
       <c r="E39">
         <v>5.5E-2</v>
       </c>
-      <c r="H39">
+      <c r="N39">
         <v>3.9E-2</v>
       </c>
-      <c r="I39">
+      <c r="O39">
         <v>5.5E-2</v>
       </c>
-      <c r="L39">
+      <c r="X39">
         <v>203.11737060546875</v>
       </c>
-      <c r="M39">
+      <c r="Y39">
         <v>203.11737060546875</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>53</v>
       </c>
@@ -2044,20 +2725,20 @@
       <c r="E40">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="H40">
+      <c r="N40">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="I40">
+      <c r="O40">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="L40">
+      <c r="X40">
         <v>3780.5404663085938</v>
       </c>
-      <c r="M40">
+      <c r="Y40">
         <v>3780.5404663085938</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>54</v>
       </c>
@@ -2073,20 +2754,20 @@
       <c r="E41">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="H41">
+      <c r="N41">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="I41">
+      <c r="O41">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="L41">
+      <c r="X41">
         <v>5965.576171875</v>
       </c>
-      <c r="M41">
+      <c r="Y41">
         <v>5998.3673095703125</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>55</v>
       </c>
@@ -2102,20 +2783,20 @@
       <c r="E42">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="H42">
+      <c r="N42">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="I42">
+      <c r="O42">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="L42">
+      <c r="X42">
         <v>1903.7246704101563</v>
       </c>
-      <c r="M42">
+      <c r="Y42">
         <v>1903.7246704101563</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>56</v>
       </c>
@@ -2138,37 +2819,61 @@
         <v>0.23</v>
       </c>
       <c r="H43">
+        <v>0.24</v>
+      </c>
+      <c r="N43">
         <v>0.04</v>
       </c>
-      <c r="I43">
+      <c r="O43">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="J43">
+      <c r="P43">
         <v>0.185</v>
       </c>
-      <c r="K43">
+      <c r="Q43">
         <v>0.188</v>
       </c>
-      <c r="L43">
+      <c r="R43">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="S43">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="T43">
+        <v>0.24</v>
+      </c>
+      <c r="X43">
         <v>2086.0977172851563</v>
       </c>
-      <c r="M43">
+      <c r="Y43">
         <v>2172.7371215820313</v>
       </c>
-      <c r="N43">
+      <c r="Z43">
         <v>430.22918701171875</v>
       </c>
-      <c r="O43">
+      <c r="AA43">
         <v>239.81475830078125</v>
       </c>
-      <c r="P43">
-        <v>8755.7296752929688</v>
-      </c>
-      <c r="Q43">
-        <v>6192.0166015625</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB43">
+        <v>6239.4027709960938</v>
+      </c>
+      <c r="AC43">
+        <v>3779.4647216796875</v>
+      </c>
+      <c r="AE43">
+        <v>585.42633056640625</v>
+      </c>
+      <c r="AF43">
+        <v>585.4949951171875</v>
+      </c>
+      <c r="AG43">
+        <v>2220.123291015625</v>
+      </c>
+      <c r="AK43">
+        <v>430.2978515625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>59</v>
       </c>
@@ -2191,37 +2896,85 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="H44">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I44">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="J44">
+        <v>0.161</v>
+      </c>
+      <c r="K44">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="N44">
         <v>2.3E-2</v>
       </c>
-      <c r="I44">
+      <c r="O44">
         <v>0.04</v>
       </c>
-      <c r="J44">
+      <c r="P44">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="K44">
+      <c r="Q44">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="L44">
+      <c r="R44">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="S44">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="T44">
+        <v>0.161</v>
+      </c>
+      <c r="U44">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="X44">
         <v>336.9293212890625</v>
       </c>
-      <c r="M44">
+      <c r="Y44">
         <v>336.9293212890625</v>
       </c>
-      <c r="N44">
+      <c r="Z44">
         <v>224.884033203125</v>
       </c>
-      <c r="O44">
+      <c r="AA44">
         <v>224.884033203125</v>
       </c>
-      <c r="P44">
-        <v>636.34490966796875</v>
-      </c>
-      <c r="Q44">
-        <v>636.34490966796875</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB44">
+        <v>74.53155517578125</v>
+      </c>
+      <c r="AC44">
+        <v>74.53155517578125</v>
+      </c>
+      <c r="AD44">
+        <v>21.026611328125</v>
+      </c>
+      <c r="AE44">
+        <v>21.026611328125</v>
+      </c>
+      <c r="AF44">
+        <v>22.14813232421875</v>
+      </c>
+      <c r="AG44">
+        <v>22.14813232421875</v>
+      </c>
+      <c r="AH44">
+        <v>54.77142333984375</v>
+      </c>
+      <c r="AI44">
+        <v>72.77679443359375</v>
+      </c>
+      <c r="AJ44">
+        <v>278.80859375</v>
+      </c>
+      <c r="AK44">
+        <v>278.80859375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>60</v>
       </c>
@@ -2244,37 +2997,61 @@
         <v>0.05</v>
       </c>
       <c r="H45">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I45">
+        <v>6.3E-2</v>
+      </c>
+      <c r="N45">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="I45">
+      <c r="O45">
         <v>2.7E-2</v>
       </c>
-      <c r="J45">
+      <c r="P45">
         <v>0.03</v>
       </c>
-      <c r="K45">
+      <c r="Q45">
         <v>0.05</v>
       </c>
-      <c r="L45">
+      <c r="R45">
+        <v>5.5E-2</v>
+      </c>
+      <c r="S45">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="X45">
         <v>189.02587890625</v>
       </c>
-      <c r="M45">
+      <c r="Y45">
         <v>199.69940185546875</v>
       </c>
-      <c r="N45">
+      <c r="Z45">
         <v>552.80303955078125</v>
       </c>
-      <c r="O45">
+      <c r="AA45">
         <v>552.80303955078125</v>
       </c>
-      <c r="P45">
-        <v>758.9111328125</v>
-      </c>
-      <c r="Q45">
-        <v>769.58465576171875</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB45">
+        <v>17.08221435546875</v>
+      </c>
+      <c r="AC45">
+        <v>17.08221435546875</v>
+      </c>
+      <c r="AD45">
+        <v>55.2215576171875</v>
+      </c>
+      <c r="AE45">
+        <v>89.30206298828125</v>
+      </c>
+      <c r="AF45">
+        <v>31.06689453125</v>
+      </c>
+      <c r="AG45">
+        <v>23.193359375</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>61</v>
       </c>
@@ -2290,20 +3067,20 @@
       <c r="E46">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H46">
+      <c r="N46">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="I46">
+      <c r="O46">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L46">
+      <c r="X46">
         <v>2745.2621459960938</v>
       </c>
-      <c r="M46">
+      <c r="Y46">
         <v>2745.2621459960938</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>62</v>
       </c>
@@ -2325,38 +3102,38 @@
       <c r="G47">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="H47">
+      <c r="N47">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="I47">
+      <c r="O47">
         <v>4.7E-2</v>
       </c>
-      <c r="J47">
+      <c r="P47">
         <v>0.05</v>
       </c>
-      <c r="K47">
+      <c r="Q47">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="L47">
+      <c r="X47">
         <v>80.72662353515625</v>
       </c>
-      <c r="M47">
+      <c r="Y47">
         <v>80.72662353515625</v>
       </c>
-      <c r="N47">
+      <c r="Z47">
         <v>74.39422607421875</v>
       </c>
-      <c r="O47">
+      <c r="AA47">
         <v>74.39422607421875</v>
       </c>
-      <c r="P47">
-        <v>207.34405517578125</v>
-      </c>
-      <c r="Q47">
-        <v>207.34405517578125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB47">
+        <v>52.22320556640625</v>
+      </c>
+      <c r="AC47">
+        <v>52.22320556640625</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>63</v>
       </c>
@@ -2372,20 +3149,20 @@
       <c r="E48">
         <v>0.08</v>
       </c>
-      <c r="H48">
+      <c r="N48">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="I48">
+      <c r="O48">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="L48">
+      <c r="X48">
         <v>119.293212890625</v>
       </c>
-      <c r="M48">
+      <c r="Y48">
         <v>152.01568603515625</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>64</v>
       </c>
@@ -2401,32 +3178,32 @@
       <c r="E49">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="H49">
+      <c r="N49">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="I49">
+      <c r="O49">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="J49">
+      <c r="P49">
         <v>5.5E-2</v>
       </c>
-      <c r="K49">
+      <c r="Q49">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="L49">
+      <c r="X49">
         <v>1620.30029296875</v>
       </c>
-      <c r="M49">
+      <c r="Y49">
         <v>1370.3079223632813</v>
       </c>
-      <c r="O49">
+      <c r="AA49">
         <v>205.57403564453125</v>
       </c>
-      <c r="Q49">
-        <v>1620.30029296875</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AC49">
+        <v>44.4183349609375</v>
+      </c>
+    </row>
+    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>65</v>
       </c>
@@ -2437,7 +3214,7 @@
         <v>76.096800000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>67</v>
       </c>
@@ -2453,20 +3230,20 @@
       <c r="E51">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H51">
+      <c r="N51">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="I51">
+      <c r="O51">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="L51">
+      <c r="X51">
         <v>2057.6248168945313</v>
       </c>
-      <c r="M51">
+      <c r="Y51">
         <v>2057.6248168945313</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>68</v>
       </c>
@@ -2477,7 +3254,7 @@
         <v>6.1219000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>72</v>
       </c>
@@ -2500,37 +3277,73 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="H53">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="I53">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="J53">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="K53">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="N53">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I53">
+      <c r="O53">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="J53">
+      <c r="P53">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="K53">
+      <c r="Q53">
         <v>0.111</v>
       </c>
-      <c r="L53">
+      <c r="R53">
+        <v>0.115</v>
+      </c>
+      <c r="S53">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="X53">
         <v>4233.2305908203125</v>
       </c>
-      <c r="M53">
+      <c r="Y53">
         <v>4233.2305908203125</v>
       </c>
-      <c r="N53">
+      <c r="Z53">
         <v>308.4259033203125</v>
       </c>
-      <c r="O53">
+      <c r="AA53">
         <v>1646.1257934570313</v>
       </c>
-      <c r="P53">
-        <v>4657.5241088867188</v>
-      </c>
-      <c r="Q53">
-        <v>6749.5651245117188</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB53">
+        <v>115.86761474609375</v>
+      </c>
+      <c r="AC53">
+        <v>870.208740234375</v>
+      </c>
+      <c r="AD53">
+        <v>7027.2674560546875</v>
+      </c>
+      <c r="AE53">
+        <v>5039.9856567382813</v>
+      </c>
+      <c r="AF53">
+        <v>317.6116943359375</v>
+      </c>
+      <c r="AG53">
+        <v>179.45098876953125</v>
+      </c>
+      <c r="AH53">
+        <v>117.12646484375</v>
+      </c>
+      <c r="AJ53">
+        <v>161.59820556640625</v>
+      </c>
+    </row>
+    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>75</v>
       </c>
@@ -2553,37 +3366,61 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="H54">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="I54">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="J54">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="K54">
+        <v>0.215</v>
+      </c>
+      <c r="N54">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I54">
+      <c r="O54">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="J54">
+      <c r="P54">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="K54">
+      <c r="Q54">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L54">
+      <c r="X54">
         <v>1530.0827026367188</v>
       </c>
-      <c r="M54">
+      <c r="Y54">
         <v>1513.2064819335938</v>
       </c>
-      <c r="N54">
+      <c r="Z54">
         <v>29.693603515625</v>
       </c>
-      <c r="O54">
+      <c r="AA54">
         <v>73.58551025390625</v>
       </c>
-      <c r="P54">
-        <v>1631.53076171875</v>
-      </c>
-      <c r="Q54">
-        <v>1754.1427612304688</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB54">
+        <v>71.75445556640625</v>
+      </c>
+      <c r="AC54">
+        <v>167.35076904296875</v>
+      </c>
+      <c r="AD54">
+        <v>101.287841796875</v>
+      </c>
+      <c r="AF54">
+        <v>37.75787353515625</v>
+      </c>
+      <c r="AH54">
+        <v>27.38189697265625</v>
+      </c>
+      <c r="AJ54">
+        <v>737.38861083984375</v>
+      </c>
+    </row>
+    <row r="55" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>77</v>
       </c>
@@ -2606,37 +3443,73 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="H55">
+        <v>0.13</v>
+      </c>
+      <c r="I55">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="J55">
+        <v>0.151</v>
+      </c>
+      <c r="K55">
+        <v>0.154</v>
+      </c>
+      <c r="L55">
+        <v>0.215</v>
+      </c>
+      <c r="M55">
+        <v>0.223</v>
+      </c>
+      <c r="N55">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="I55">
+      <c r="O55">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="J55">
+      <c r="P55">
         <v>0.13300000000000001</v>
       </c>
-      <c r="K55">
+      <c r="Q55">
         <v>0.13600000000000001</v>
       </c>
-      <c r="L55">
+      <c r="X55">
         <v>214.17236328125</v>
       </c>
-      <c r="M55">
+      <c r="Y55">
         <v>309.53216552734375</v>
       </c>
-      <c r="N55">
+      <c r="Z55">
         <v>499.83978271484375</v>
       </c>
-      <c r="O55">
+      <c r="AA55">
         <v>104.8431396484375</v>
       </c>
-      <c r="P55">
-        <v>834.5947265625</v>
-      </c>
-      <c r="Q55">
-        <v>1475.8377075195313</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB55">
+        <v>120.58258056640625</v>
+      </c>
+      <c r="AC55">
+        <v>1061.46240234375</v>
+      </c>
+      <c r="AD55">
+        <v>425.07171630859375</v>
+      </c>
+      <c r="AF55">
+        <v>832.8094482421875</v>
+      </c>
+      <c r="AH55">
+        <v>88.2720947265625</v>
+      </c>
+      <c r="AJ55">
+        <v>170.7305908203125</v>
+      </c>
+      <c r="AL55">
+        <v>236.88507080078125</v>
+      </c>
+      <c r="AN55">
+        <v>641.448974609375</v>
+      </c>
+    </row>
+    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>78</v>
       </c>
@@ -2659,37 +3532,61 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="H56">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="I56">
+        <v>0.113</v>
+      </c>
+      <c r="N56">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="I56">
+      <c r="O56">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="J56">
+      <c r="P56">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="K56">
+      <c r="Q56">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="L56">
+      <c r="R56">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="S56">
+        <v>0.113</v>
+      </c>
+      <c r="X56">
         <v>100.30364990234375</v>
       </c>
-      <c r="M56">
+      <c r="Y56">
         <v>100.30364990234375</v>
       </c>
-      <c r="N56">
+      <c r="Z56">
         <v>88.60015869140625</v>
       </c>
-      <c r="O56">
+      <c r="AA56">
         <v>88.60015869140625</v>
       </c>
-      <c r="P56">
-        <v>208.770751953125</v>
-      </c>
-      <c r="Q56">
-        <v>208.770751953125</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AB56">
+        <v>19.866943359375</v>
+      </c>
+      <c r="AC56">
+        <v>19.866943359375</v>
+      </c>
+      <c r="AD56">
+        <v>249.07684326171875</v>
+      </c>
+      <c r="AE56">
+        <v>249.07684326171875</v>
+      </c>
+      <c r="AF56">
+        <v>169.7998046875</v>
+      </c>
+      <c r="AG56">
+        <v>169.7998046875</v>
+      </c>
+    </row>
+    <row r="57" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>79</v>
       </c>
@@ -2699,29 +3596,29 @@
       <c r="C57">
         <v>5.5084999999999997</v>
       </c>
-      <c r="H57">
+      <c r="N57">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="I57">
+      <c r="O57">
         <v>0.03</v>
       </c>
-      <c r="J57">
+      <c r="P57">
         <v>0.05</v>
       </c>
-      <c r="K57">
+      <c r="Q57">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="M57">
+      <c r="Y57">
         <v>25.12359619140625</v>
       </c>
-      <c r="O57">
+      <c r="AA57">
         <v>17.23480224609375</v>
       </c>
-      <c r="Q57">
-        <v>102.08892822265625</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="AC57">
+        <v>59.73052978515625</v>
+      </c>
+    </row>
+    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>80</v>
       </c>
@@ -2737,16 +3634,16 @@
       <c r="E58">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="H58">
+      <c r="N58">
         <v>0.04</v>
       </c>
-      <c r="I58">
+      <c r="O58">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="L58">
+      <c r="X58">
         <v>635.03265380859375</v>
       </c>
-      <c r="M58">
+      <c r="Y58">
         <v>635.03265380859375</v>
       </c>
     </row>

</xml_diff>